<commit_message>
invert forward and reverse primers for project GEP00006
</commit_message>
<xml_diff>
--- a/data/GEP00006/GEP00006.xlsx
+++ b/data/GEP00006/GEP00006.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="35200" yWindow="0" windowWidth="25000" windowHeight="15220" tabRatio="685"/>
+    <workbookView xWindow="35200" yWindow="0" windowWidth="25000" windowHeight="15220" tabRatio="685" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -952,9 +952,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -975,9 +981,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="10">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1259,7 +1271,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
@@ -1592,10 +1604,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1699,28 +1711,28 @@
         <v>20</v>
       </c>
       <c r="I2">
-        <v>352</v>
+        <v>353.1</v>
       </c>
       <c r="J2" t="s">
+        <v>74</v>
+      </c>
+      <c r="K2" s="5">
+        <v>10672758</v>
+      </c>
+      <c r="L2" s="6">
+        <v>10672777</v>
+      </c>
+      <c r="M2">
+        <v>352.1</v>
+      </c>
+      <c r="N2" t="s">
         <v>73</v>
       </c>
-      <c r="K2" s="5">
+      <c r="O2" s="5">
         <v>10672928</v>
       </c>
-      <c r="L2" s="5">
+      <c r="P2" s="5">
         <v>10672946</v>
-      </c>
-      <c r="M2">
-        <v>353</v>
-      </c>
-      <c r="N2" t="s">
-        <v>74</v>
-      </c>
-      <c r="O2" s="5">
-        <v>10672758</v>
-      </c>
-      <c r="P2" s="6">
-        <v>10672777</v>
       </c>
       <c r="Q2" t="s">
         <v>75</v>
@@ -1752,32 +1764,44 @@
         <v>20</v>
       </c>
       <c r="I3">
-        <v>352</v>
+        <v>353.1</v>
       </c>
       <c r="J3" t="s">
+        <v>74</v>
+      </c>
+      <c r="K3" s="5">
+        <v>10672758</v>
+      </c>
+      <c r="L3" s="6">
+        <v>10672777</v>
+      </c>
+      <c r="M3">
+        <v>352.1</v>
+      </c>
+      <c r="N3" t="s">
         <v>73</v>
       </c>
-      <c r="K3" s="5">
+      <c r="O3" s="5">
         <v>10672928</v>
       </c>
-      <c r="L3" s="5">
+      <c r="P3" s="5">
         <v>10672946</v>
-      </c>
-      <c r="M3">
-        <v>353</v>
-      </c>
-      <c r="N3" t="s">
-        <v>74</v>
-      </c>
-      <c r="O3" s="5">
-        <v>10672758</v>
-      </c>
-      <c r="P3" s="6">
-        <v>10672777</v>
       </c>
       <c r="Q3" t="s">
         <v>75</v>
       </c>
+    </row>
+    <row r="6" spans="1:17" ht="15">
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="6"/>
+    </row>
+    <row r="7" spans="1:17" ht="15">
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>